<commit_message>
Hecha la interfaz de edicion del mensaje
</commit_message>
<xml_diff>
--- a/documentos/Check list.xlsx
+++ b/documentos/Check list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fbfffc4df1949f3a/Desktop/Crombieversario-Autom-tico/documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_F1A49E3F63D378C652BFA1F4C32528E350C29C20" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C151C96-FA6A-4D1E-A0CD-C606DB5E1D7B}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_F1A49E3F63D378C652BFA1F4C32528E350C29C20" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B5C0B7B-A0CC-42F4-93FC-C632C9A10AF0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4440" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Se puede hacer el documento che" sheetId="1" r:id="rId1"/>
@@ -260,7 +260,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\.m"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -280,8 +280,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -290,14 +311,23 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -310,10 +340,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -324,16 +357,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bueno" xfId="1" builtinId="26"/>
+    <cellStyle name="Incorrecto" xfId="2" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
@@ -405,6 +448,7 @@
         <name val="Arial"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="164" formatCode="d\.m"/>
     </dxf>
     <dxf>
       <font>
@@ -422,7 +466,6 @@
         <name val="Arial"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="d\.m"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -438,11 +481,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2B703D67-400D-421B-A8A9-46A6F8E35D28}" name="Tabla1" displayName="Tabla1" ref="A1:G42" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2B703D67-400D-421B-A8A9-46A6F8E35D28}" name="Tabla1" displayName="Tabla1" ref="A1:G42" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:G42" xr:uid="{2B703D67-400D-421B-A8A9-46A6F8E35D28}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{37FE3DB3-00C3-4410-B567-ADDA89DD4B6F}" name="ID" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{BD914BBE-D36F-4096-BB34-23E825D5837C}" name="Categoría" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{37FE3DB3-00C3-4410-B567-ADDA89DD4B6F}" name="ID" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{BD914BBE-D36F-4096-BB34-23E825D5837C}" name="Categoría" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{DB5DDB5E-7DEC-4FE4-B145-8FE0EE08CD70}" name="Tarea/Funcionalidad" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{FF30D2FE-99A8-48D7-91F4-7F0D585FFAEF}" name="Estado" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{78381461-46B3-45E4-8C6A-C2477A7E2FB9}" name="Notas/Comentarios"/>
@@ -656,8 +699,8 @@
   </sheetPr>
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -669,7 +712,7 @@
     <col min="7" max="7" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -692,13 +735,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:7" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="9"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D2" s="8"/>
+    </row>
+    <row r="3" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -708,9 +751,9 @@
       <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D3" s="9"/>
+    </row>
+    <row r="4" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -720,9 +763,9 @@
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D4" s="9"/>
+    </row>
+    <row r="5" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -732,9 +775,9 @@
       <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D5" s="9"/>
+    </row>
+    <row r="6" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -744,15 +787,15 @@
       <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="D6" s="9"/>
+    </row>
+    <row r="7" spans="1:7" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="9"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>45658</v>
       </c>
@@ -762,12 +805,12 @@
       <c r="C8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="6"/>
+      <c r="D8" s="9"/>
       <c r="E8" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>45689</v>
       </c>
@@ -777,9 +820,9 @@
       <c r="C9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>45717</v>
       </c>
@@ -789,9 +832,9 @@
       <c r="C10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D10" s="9"/>
+    </row>
+    <row r="11" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>45748</v>
       </c>
@@ -801,12 +844,12 @@
       <c r="C11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="6"/>
+      <c r="D11" s="9"/>
       <c r="E11" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>45778</v>
       </c>
@@ -816,9 +859,9 @@
       <c r="C12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="6"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D12" s="9"/>
+    </row>
+    <row r="13" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>45809</v>
       </c>
@@ -828,18 +871,18 @@
       <c r="C13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="6"/>
+      <c r="D13" s="9"/>
       <c r="E13" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
+    <row r="14" spans="1:7" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="9"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>45659</v>
       </c>
@@ -849,9 +892,9 @@
       <c r="C15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D15" s="9"/>
+    </row>
+    <row r="16" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>45690</v>
       </c>
@@ -861,12 +904,12 @@
       <c r="C16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="4"/>
+      <c r="D16" s="10"/>
       <c r="E16" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>45718</v>
       </c>
@@ -876,9 +919,9 @@
       <c r="C17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D17" s="9"/>
+    </row>
+    <row r="18" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>45749</v>
       </c>
@@ -888,9 +931,9 @@
       <c r="C18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D18" s="12"/>
+    </row>
+    <row r="19" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>45779</v>
       </c>
@@ -900,9 +943,9 @@
       <c r="C19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D19" s="12"/>
+    </row>
+    <row r="20" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>45810</v>
       </c>
@@ -912,15 +955,15 @@
       <c r="C20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
+      <c r="D20" s="12"/>
+    </row>
+    <row r="21" spans="1:5" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="9"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D21" s="8"/>
+    </row>
+    <row r="22" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>45660</v>
       </c>
@@ -930,12 +973,12 @@
       <c r="C22" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="4"/>
+      <c r="D22" s="9"/>
       <c r="E22" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>45691</v>
       </c>
@@ -945,12 +988,12 @@
       <c r="C23" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="4"/>
+      <c r="D23" s="12"/>
       <c r="E23" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>45719</v>
       </c>
@@ -960,15 +1003,15 @@
       <c r="C24" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="4"/>
-    </row>
-    <row r="25" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="7" t="s">
+      <c r="D24" s="12"/>
+    </row>
+    <row r="25" spans="1:5" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="9"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>45661</v>
       </c>
@@ -980,7 +1023,7 @@
       </c>
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>45692</v>
       </c>
@@ -990,9 +1033,9 @@
       <c r="C27" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D27" s="9"/>
+    </row>
+    <row r="28" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>45720</v>
       </c>
@@ -1002,9 +1045,9 @@
       <c r="C28" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D28" s="9"/>
+    </row>
+    <row r="29" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>45751</v>
       </c>
@@ -1014,15 +1057,15 @@
       <c r="C29" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="7" t="s">
+      <c r="D29" s="11"/>
+    </row>
+    <row r="30" spans="1:5" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D30" s="9"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D30" s="8"/>
+    </row>
+    <row r="31" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>45662</v>
       </c>
@@ -1032,9 +1075,9 @@
       <c r="C31" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D31" s="4"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D31" s="12"/>
+    </row>
+    <row r="32" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>45693</v>
       </c>
@@ -1044,9 +1087,9 @@
       <c r="C32" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D32" s="4"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D32" s="12"/>
+    </row>
+    <row r="33" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>45721</v>
       </c>
@@ -1056,9 +1099,9 @@
       <c r="C33" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D33" s="4"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D33" s="12"/>
+    </row>
+    <row r="34" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>45752</v>
       </c>
@@ -1068,15 +1111,15 @@
       <c r="C34" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D34" s="4"/>
-    </row>
-    <row r="35" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="7" t="s">
+      <c r="D34" s="12"/>
+    </row>
+    <row r="35" spans="1:4" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D35" s="9"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D35" s="8"/>
+    </row>
+    <row r="36" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>45663</v>
       </c>
@@ -1086,9 +1129,9 @@
       <c r="C36" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D36" s="4"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D36" s="12"/>
+    </row>
+    <row r="37" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>45694</v>
       </c>
@@ -1098,9 +1141,9 @@
       <c r="C37" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D37" s="4"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D37" s="12"/>
+    </row>
+    <row r="38" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>45722</v>
       </c>
@@ -1110,9 +1153,9 @@
       <c r="C38" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D38" s="12"/>
+    </row>
+    <row r="39" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>45753</v>
       </c>
@@ -1122,9 +1165,9 @@
       <c r="C39" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D39" s="4"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D39" s="12"/>
+    </row>
+    <row r="40" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>45783</v>
       </c>
@@ -1134,9 +1177,9 @@
       <c r="C40" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D40" s="4"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D40" s="12"/>
+    </row>
+    <row r="41" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>45814</v>
       </c>
@@ -1146,7 +1189,7 @@
       <c r="C41" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D41" s="4"/>
+      <c r="D41" s="12"/>
     </row>
     <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
@@ -1158,7 +1201,7 @@
       <c r="C42" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D42" s="4"/>
+      <c r="D42" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Anda el tracking de mails abiertos
</commit_message>
<xml_diff>
--- a/documentos/Check list.xlsx
+++ b/documentos/Check list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fbfffc4df1949f3a/Desktop/Crombieversario-Autom-tico/documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_F1A49E3F63D378C652BFA1F4C32528E350C29C20" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B5C0B7B-A0CC-42F4-93FC-C632C9A10AF0}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="11_F1A49E3F63D378C652BFA1F4C32528E350C29C20" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DFF08B34-9310-4DFF-B7AF-2E0424DB0446}"/>
   <bookViews>
-    <workbookView xWindow="-4440" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Se puede hacer el documento che" sheetId="1" r:id="rId1"/>
@@ -365,13 +365,13 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
@@ -699,8 +699,8 @@
   </sheetPr>
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -904,7 +904,7 @@
       <c r="C16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="10"/>
+      <c r="D16" s="12"/>
       <c r="E16" s="1" t="s">
         <v>33</v>
       </c>
@@ -931,7 +931,7 @@
       <c r="C18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="12"/>
+      <c r="D18" s="9"/>
     </row>
     <row r="19" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
@@ -943,7 +943,7 @@
       <c r="C19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="12"/>
+      <c r="D19" s="11"/>
     </row>
     <row r="20" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
@@ -955,7 +955,7 @@
       <c r="C20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="12"/>
+      <c r="D20" s="11"/>
     </row>
     <row r="21" spans="1:5" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
@@ -988,7 +988,7 @@
       <c r="C23" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="12"/>
+      <c r="D23" s="9"/>
       <c r="E23" s="1" t="s">
         <v>45</v>
       </c>
@@ -1003,7 +1003,7 @@
       <c r="C24" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="12"/>
+      <c r="D24" s="9"/>
     </row>
     <row r="25" spans="1:5" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
@@ -1057,7 +1057,7 @@
       <c r="C29" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="11"/>
+      <c r="D29" s="10"/>
     </row>
     <row r="30" spans="1:5" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
@@ -1075,7 +1075,7 @@
       <c r="C31" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D31" s="12"/>
+      <c r="D31" s="11"/>
     </row>
     <row r="32" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
@@ -1087,7 +1087,7 @@
       <c r="C32" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D32" s="12"/>
+      <c r="D32" s="11"/>
     </row>
     <row r="33" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
@@ -1099,7 +1099,7 @@
       <c r="C33" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D33" s="12"/>
+      <c r="D33" s="11"/>
     </row>
     <row r="34" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
@@ -1111,7 +1111,7 @@
       <c r="C34" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D34" s="12"/>
+      <c r="D34" s="11"/>
     </row>
     <row r="35" spans="1:4" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
@@ -1129,7 +1129,7 @@
       <c r="C36" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D36" s="12"/>
+      <c r="D36" s="11"/>
     </row>
     <row r="37" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
@@ -1141,7 +1141,7 @@
       <c r="C37" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D37" s="12"/>
+      <c r="D37" s="11"/>
     </row>
     <row r="38" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
@@ -1153,7 +1153,7 @@
       <c r="C38" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D38" s="12"/>
+      <c r="D38" s="11"/>
     </row>
     <row r="39" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
@@ -1165,7 +1165,7 @@
       <c r="C39" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D39" s="12"/>
+      <c r="D39" s="11"/>
     </row>
     <row r="40" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
@@ -1177,7 +1177,7 @@
       <c r="C40" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D40" s="12"/>
+      <c r="D40" s="11"/>
     </row>
     <row r="41" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
@@ -1189,7 +1189,7 @@
       <c r="C41" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D41" s="12"/>
+      <c r="D41" s="11"/>
     </row>
     <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
@@ -1201,7 +1201,7 @@
       <c r="C42" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D42" s="12"/>
+      <c r="D42" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Actualice el Check list
</commit_message>
<xml_diff>
--- a/documentos/Check list.xlsx
+++ b/documentos/Check list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fbfffc4df1949f3a/Desktop/Crombieversario-Autom-tico/documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="11_F1A49E3F63D378C652BFA1F4C32528E350C29C20" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DFF08B34-9310-4DFF-B7AF-2E0424DB0446}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="11_F1A49E3F63D378C652BFA1F4C32528E350C29C20" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96552A5F-8A14-4EB5-BE51-45455DB3269D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -699,8 +699,8 @@
   </sheetPr>
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -943,7 +943,7 @@
       <c r="C19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="11"/>
+      <c r="D19" s="9"/>
     </row>
     <row r="20" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
@@ -955,7 +955,7 @@
       <c r="C20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="11"/>
+      <c r="D20" s="9"/>
     </row>
     <row r="21" spans="1:5" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
@@ -1057,7 +1057,7 @@
       <c r="C29" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="10"/>
+      <c r="D29" s="9"/>
     </row>
     <row r="30" spans="1:5" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
@@ -1111,7 +1111,7 @@
       <c r="C34" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D34" s="11"/>
+      <c r="D34" s="10"/>
     </row>
     <row r="35" spans="1:4" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">

</xml_diff>